<commit_message>
add 45Q incentives; allow fixed parameter
</commit_message>
<xml_diff>
--- a/CCU/EtOH/analyses/parameter_distributions/10_full_samples.xlsx
+++ b/CCU/EtOH/analyses/parameter_distributions/10_full_samples.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK12"/>
+  <dimension ref="A1:BL12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,82 +659,87 @@
       </c>
       <c r="AV1" t="inlineStr">
         <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>C3</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>C3</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>D1</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>D1</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>D2</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>D2</t>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -926,132 +931,137 @@
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>CO2 recovery</t>
+          <t>MEA unit price</t>
         </is>
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>MEA unit price</t>
+          <t>Catalyst_MeOH unit price</t>
         </is>
       </c>
       <c r="AN2" t="inlineStr">
         <is>
-          <t>Catalyst_MeOH unit price</t>
+          <t xml:space="preserve">Heat integration split recycled </t>
         </is>
       </c>
       <c r="AO2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Heat integration split recycled </t>
+          <t>MeOH conversion</t>
         </is>
       </c>
       <c r="AP2" t="inlineStr">
         <is>
-          <t>MeOH conversion</t>
+          <t>MeOH conversion WHSV</t>
         </is>
       </c>
       <c r="AQ2" t="inlineStr">
         <is>
-          <t>MeOH conversion WHSV</t>
+          <t>MeOH conversion catalyst density</t>
         </is>
       </c>
       <c r="AR2" t="inlineStr">
         <is>
-          <t>MeOH conversion catalyst density</t>
+          <t>MeOH conversion catalyst longevity</t>
         </is>
       </c>
       <c r="AS2" t="inlineStr">
         <is>
-          <t>MeOH conversion catalyst longevity</t>
+          <t>MeOH conversion porosity</t>
         </is>
       </c>
       <c r="AT2" t="inlineStr">
         <is>
-          <t>MeOH conversion porosity</t>
+          <t>Methanol unit price</t>
         </is>
       </c>
       <c r="AU2" t="inlineStr">
         <is>
-          <t>Methanol unit price</t>
+          <t>Methanol GWP</t>
         </is>
       </c>
       <c r="AV2" t="inlineStr">
         <is>
-          <t>Methanol GWP</t>
+          <t>Electrolyzer stack longevity</t>
         </is>
       </c>
       <c r="AW2" t="inlineStr">
         <is>
-          <t>Electrolyzer stack longevity</t>
+          <t>Electrolyzer stack F_BM</t>
         </is>
       </c>
       <c r="AX2" t="inlineStr">
         <is>
-          <t>Electrolyzer stack F_BM</t>
+          <t>Electrolyzer mechanical BOP F_BM</t>
         </is>
       </c>
       <c r="AY2" t="inlineStr">
         <is>
-          <t>Electrolyzer mechanical BOP F_BM</t>
+          <t>Electrolyzer electrical BOP F_BM</t>
         </is>
       </c>
       <c r="AZ2" t="inlineStr">
         <is>
-          <t>Electrolyzer electrical BOP F_BM</t>
+          <t>Electrolyzer base_power_per_hydrogen_flow</t>
         </is>
       </c>
       <c r="BA2" t="inlineStr">
         <is>
-          <t>Electrolyzer base_power_per_hydrogen_flow</t>
+          <t>Oxygen unit price</t>
         </is>
       </c>
       <c r="BB2" t="inlineStr">
         <is>
-          <t>Oxygen unit price</t>
+          <t>Oxygen GWP</t>
         </is>
       </c>
       <c r="BC2" t="inlineStr">
         <is>
-          <t>Oxygen GWP</t>
+          <t>Hydrogen unit price (conventional)</t>
         </is>
       </c>
       <c r="BD2" t="inlineStr">
         <is>
-          <t>Hydrogen unit price (conventional)</t>
+          <t>Hydrogen GWP (conventional)</t>
         </is>
       </c>
       <c r="BE2" t="inlineStr">
         <is>
-          <t>Hydrogen GWP (conventional)</t>
+          <t>Hydrogen unit price (renewable)</t>
         </is>
       </c>
       <c r="BF2" t="inlineStr">
         <is>
-          <t>Hydrogen unit price (renewable)</t>
+          <t>Hydrogen GWP (renewable)</t>
         </is>
       </c>
       <c r="BG2" t="inlineStr">
         <is>
-          <t>Hydrogen GWP (renewable)</t>
+          <t>Electricity unit price (conventional)</t>
         </is>
       </c>
       <c r="BH2" t="inlineStr">
         <is>
-          <t>Electricity unit price (conventional)</t>
+          <t>Electricity GWP (conventional)</t>
         </is>
       </c>
       <c r="BI2" t="inlineStr">
         <is>
-          <t>Electricity GWP (conventional)</t>
+          <t>Electricity unit price (renewable)</t>
         </is>
       </c>
       <c r="BJ2" t="inlineStr">
         <is>
-          <t>Electricity unit price (renewable)</t>
+          <t>Electricity GWP (renewable)</t>
         </is>
       </c>
       <c r="BK2" t="inlineStr">
         <is>
-          <t>Electricity GWP (renewable)</t>
+          <t>CCU credit</t>
+        </is>
+      </c>
+      <c r="BL2" t="inlineStr">
+        <is>
+          <t>CCU credit years</t>
         </is>
       </c>
     </row>
@@ -1168,82 +1178,85 @@
         <v>0.3124138832473172</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.8989763902430679</v>
+        <v>1.610441603120029</v>
       </c>
       <c r="AM3" t="n">
-        <v>1.553856465691039</v>
+        <v>35.05433310351172</v>
       </c>
       <c r="AN3" t="n">
-        <v>27.93871174579434</v>
+        <v>0.5457425662086453</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.6268135969632463</v>
+        <v>0.2193847589371362</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.22826414373153</v>
+        <v>3.148470948021103</v>
       </c>
       <c r="AQ3" t="n">
-        <v>2.898146953330186</v>
+        <v>1775.97755265085</v>
       </c>
       <c r="AR3" t="n">
-        <v>1785.602920965986</v>
+        <v>7931.094889518778</v>
       </c>
       <c r="AS3" t="n">
-        <v>8657.280788254971</v>
+        <v>0.5490411458812133</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.5438715032930874</v>
+        <v>0.37367340144707</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.321251402619748</v>
+        <v>0.4902450518123029</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.6247532358246292</v>
+        <v>10.77160751421775</v>
       </c>
       <c r="AW3" t="n">
-        <v>9.796436803469035</v>
+        <v>0.9894401171503726</v>
       </c>
       <c r="AX3" t="n">
-        <v>1.090619237946626</v>
+        <v>1.490153018184499</v>
       </c>
       <c r="AY3" t="n">
-        <v>1.233579593440338</v>
+        <v>0.9385931689219965</v>
       </c>
       <c r="AZ3" t="n">
-        <v>1.024528282245301</v>
+        <v>56.57737896924907</v>
       </c>
       <c r="BA3" t="n">
-        <v>63.05761323125082</v>
+        <v>0.2501250524832314</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.2647722550268049</v>
+        <v>0.1986943096418544</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.1535358553369024</v>
+        <v>0.9724759901946821</v>
       </c>
       <c r="BD3" t="n">
-        <v>1.053271526463462</v>
+        <v>12.0146966066097</v>
       </c>
       <c r="BE3" t="n">
-        <v>10.39448988398291</v>
+        <v>3.695731094996853</v>
       </c>
       <c r="BF3" t="n">
-        <v>4.3680290543636</v>
+        <v>0.6627996661674525</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.2536245311700845</v>
+        <v>0.08294154046556321</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.101345933454175</v>
+        <v>0.4839756722869181</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.4903419431916636</v>
+        <v>0</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.03616392596891307</v>
+        <v>0.02164267887190791</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.02004597357135025</v>
+        <v>74.07127953482455</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>12.8647189938306</v>
       </c>
     </row>
     <row r="4">
@@ -1359,82 +1372,85 @@
         <v>0.3304005894647825</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.7966377394717724</v>
+        <v>1.374653351742964</v>
       </c>
       <c r="AM4" t="n">
-        <v>1.285472858897804</v>
+        <v>28.99971444356492</v>
       </c>
       <c r="AN4" t="n">
-        <v>34.11121295379142</v>
+        <v>0.6160891480559249</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.6366292149446208</v>
+        <v>0.2228202252306173</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.186106240824027</v>
+        <v>2.566982632055544</v>
       </c>
       <c r="AQ4" t="n">
-        <v>3.161914126490375</v>
+        <v>1937.613448346334</v>
       </c>
       <c r="AR4" t="n">
-        <v>1582.865734174084</v>
+        <v>7030.599125762525</v>
       </c>
       <c r="AS4" t="n">
-        <v>7782.997490954719</v>
+        <v>0.4935944628966716</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.4616960946326234</v>
+        <v>0.337227592694029</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.3822053880167865</v>
+        <v>0.6519916413437414</v>
       </c>
       <c r="AV4" t="n">
-        <v>0.574830409926574</v>
+        <v>9.91086913666507</v>
       </c>
       <c r="AW4" t="n">
-        <v>10.61971124995502</v>
+        <v>1.072590836245457</v>
       </c>
       <c r="AX4" t="n">
-        <v>0.8768729879869696</v>
+        <v>1.198103686556453</v>
       </c>
       <c r="AY4" t="n">
-        <v>1.532974113370428</v>
+        <v>1.166393347129673</v>
       </c>
       <c r="AZ4" t="n">
-        <v>1.040686313282827</v>
+        <v>57.46967160894422</v>
       </c>
       <c r="BA4" t="n">
-        <v>58.4411526901719</v>
+        <v>0.2318133471085047</v>
       </c>
       <c r="BB4" t="n">
-        <v>0.2313154804771817</v>
+        <v>0.1735871823059199</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.1667309901824082</v>
+        <v>1.008739037829258</v>
       </c>
       <c r="BD4" t="n">
-        <v>0.9605062879867671</v>
+        <v>9.550657567064762</v>
       </c>
       <c r="BE4" t="n">
-        <v>11.07972405884287</v>
+        <v>4.037414950784498</v>
       </c>
       <c r="BF4" t="n">
-        <v>3.95275288051328</v>
+        <v>0.5212509579126134</v>
       </c>
       <c r="BG4" t="n">
-        <v>0.7677030232571573</v>
+        <v>0.09968215604725696</v>
       </c>
       <c r="BH4" t="n">
-        <v>0.08419882830363538</v>
+        <v>0.3993009170013498</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.4088044828491965</v>
+        <v>0</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.04338408756227312</v>
+        <v>0.01804378407058523</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.02157156911543484</v>
+        <v>87.83610107529771</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>13.95274385466979</v>
       </c>
     </row>
     <row r="5">
@@ -1550,82 +1566,85 @@
         <v>0.3478657624522924</v>
       </c>
       <c r="AL5" t="n">
-        <v>0.770645845655526</v>
+        <v>1.314768028390332</v>
       </c>
       <c r="AM5" t="n">
-        <v>1.57787124674452</v>
+        <v>35.59609622838455</v>
       </c>
       <c r="AN5" t="n">
-        <v>30.01606531223378</v>
+        <v>0.5744787627083249</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.5964506616296823</v>
+        <v>0.2087577315703888</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.212899483745142</v>
+        <v>2.936544603381268</v>
       </c>
       <c r="AQ5" t="n">
-        <v>2.594209993306887</v>
+        <v>1589.725707208001</v>
       </c>
       <c r="AR5" t="n">
-        <v>1686.565193209569</v>
+        <v>7491.199990571404</v>
       </c>
       <c r="AS5" t="n">
-        <v>7897.722949377312</v>
+        <v>0.5008703037403166</v>
       </c>
       <c r="AT5" t="n">
-        <v>0.4724959109974667</v>
+        <v>0.3416436480382924</v>
       </c>
       <c r="AU5" t="n">
-        <v>0.3654427405680914</v>
+        <v>0.6105354633924327</v>
       </c>
       <c r="AV5" t="n">
-        <v>0.5166684029622621</v>
+        <v>8.908075913142451</v>
       </c>
       <c r="AW5" t="n">
-        <v>11.10946650792122</v>
+        <v>1.122056117300043</v>
       </c>
       <c r="AX5" t="n">
-        <v>0.9987520412730544</v>
+        <v>1.364631501937441</v>
       </c>
       <c r="AY5" t="n">
-        <v>1.435879298983865</v>
+        <v>1.092516857922506</v>
       </c>
       <c r="AZ5" t="n">
-        <v>1.14255743818738</v>
+        <v>63.09528618653049</v>
       </c>
       <c r="BA5" t="n">
-        <v>52.78773579159726</v>
+        <v>0.2093884387428838</v>
       </c>
       <c r="BB5" t="n">
-        <v>0.2284092034769482</v>
+        <v>0.1714062109570489</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.1861973496751979</v>
+        <v>1.05125004502594</v>
       </c>
       <c r="BD5" t="n">
-        <v>1.003906276395128</v>
+        <v>10.56167962869034</v>
       </c>
       <c r="BE5" t="n">
-        <v>10.96014393303059</v>
+        <v>3.962748497191042</v>
       </c>
       <c r="BF5" t="n">
-        <v>4.040904504544179</v>
+        <v>0.5562972997006265</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.5689023543667168</v>
+        <v>0.09078781509376259</v>
       </c>
       <c r="BH5" t="n">
-        <v>0.09081841764602103</v>
+        <v>0.4386314325985388</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.4489114780143248</v>
+        <v>0</v>
       </c>
       <c r="BJ5" t="n">
-        <v>0.03009600913105431</v>
+        <v>0.01981402385718399</v>
       </c>
       <c r="BK5" t="n">
-        <v>0.02028473713928789</v>
+        <v>62.15276524669687</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>13.03500049392157</v>
       </c>
     </row>
     <row r="6">
@@ -1741,82 +1760,85 @@
         <v>0.3898367736965631</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.7120240512808846</v>
+        <v>1.179703414151158</v>
       </c>
       <c r="AM6" t="n">
-        <v>1.652565373089038</v>
+        <v>37.28116357119865</v>
       </c>
       <c r="AN6" t="n">
-        <v>32.2641519392805</v>
+        <v>0.597935546608431</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.691665700045193</v>
+        <v>0.2420829950158175</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.2409853329592584</v>
+        <v>3.323935627024253</v>
       </c>
       <c r="AQ6" t="n">
-        <v>2.780600448756384</v>
+        <v>1703.945334520654</v>
       </c>
       <c r="AR6" t="n">
-        <v>1958.49152616936</v>
+        <v>8699.012502715061</v>
       </c>
       <c r="AS6" t="n">
-        <v>7608.637023102484</v>
+        <v>0.4825365945650992</v>
       </c>
       <c r="AT6" t="n">
-        <v>0.4415844299057974</v>
+        <v>0.3290039135592568</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.3629253605466637</v>
+        <v>0.6043096595951036</v>
       </c>
       <c r="AV6" t="n">
-        <v>0.5153869898336527</v>
+        <v>8.885982583338841</v>
       </c>
       <c r="AW6" t="n">
-        <v>10.03796592448317</v>
+        <v>1.013834558372801</v>
       </c>
       <c r="AX6" t="n">
-        <v>1.15749251088024</v>
+        <v>1.581524420806664</v>
       </c>
       <c r="AY6" t="n">
-        <v>1.309885452261514</v>
+        <v>0.9966519745468041</v>
       </c>
       <c r="AZ6" t="n">
-        <v>1.194401682103574</v>
+        <v>65.95827346199394</v>
       </c>
       <c r="BA6" t="n">
-        <v>55.4467671357443</v>
+        <v>0.2199357829956745</v>
       </c>
       <c r="BB6" t="n">
-        <v>0.2384462135262008</v>
+        <v>0.1789383324114011</v>
       </c>
       <c r="BC6" t="n">
-        <v>0.1420508098168775</v>
+        <v>0.9409126331199501</v>
       </c>
       <c r="BD6" t="n">
-        <v>0.9804345684765124</v>
+        <v>10.01489573772551</v>
       </c>
       <c r="BE6" t="n">
-        <v>10.23353580632046</v>
+        <v>3.637120146400111</v>
       </c>
       <c r="BF6" t="n">
-        <v>4.180284308266902</v>
+        <v>0.6037424768687916</v>
       </c>
       <c r="BG6" t="n">
-        <v>0.4395763171271741</v>
+        <v>0.086653942166265</v>
       </c>
       <c r="BH6" t="n">
-        <v>0.08960734613618085</v>
+        <v>0.4333856775346247</v>
       </c>
       <c r="BI6" t="n">
-        <v>0.3541061472490304</v>
+        <v>0</v>
       </c>
       <c r="BJ6" t="n">
-        <v>0.04006695985885653</v>
+        <v>0.0156295127061641</v>
       </c>
       <c r="BK6" t="n">
-        <v>0.01938287559140987</v>
+        <v>81.73756212032436</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>12.39181050235996</v>
       </c>
     </row>
     <row r="7">
@@ -1932,82 +1954,85 @@
         <v>0.3755015056236315</v>
       </c>
       <c r="AL7" t="n">
-        <v>0.928913239489267</v>
+        <v>1.679416103783271</v>
       </c>
       <c r="AM7" t="n">
-        <v>1.370131114084075</v>
+        <v>30.90956824459912</v>
       </c>
       <c r="AN7" t="n">
-        <v>28.60730201904306</v>
+        <v>0.556183449416613</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.6523813799291522</v>
+        <v>0.2283334829752033</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.2217244475664873</v>
+        <v>3.058268242296375</v>
       </c>
       <c r="AQ7" t="n">
-        <v>2.547237872971682</v>
+        <v>1560.941303704969</v>
       </c>
       <c r="AR7" t="n">
-        <v>1756.321412914459</v>
+        <v>7801.035503897236</v>
       </c>
       <c r="AS7" t="n">
-        <v>6862.654521658066</v>
+        <v>0.4352266946764374</v>
       </c>
       <c r="AT7" t="n">
-        <v>0.4831424178488715</v>
+        <v>0.345997014974413</v>
       </c>
       <c r="AU7" t="n">
-        <v>0.3433357357122753</v>
+        <v>0.5528954941372662</v>
       </c>
       <c r="AV7" t="n">
-        <v>0.5672884499260719</v>
+        <v>9.780835343552964</v>
       </c>
       <c r="AW7" t="n">
-        <v>9.36348191912008</v>
+        <v>0.9457116738311282</v>
       </c>
       <c r="AX7" t="n">
-        <v>1.060475796708869</v>
+        <v>1.448966930156673</v>
       </c>
       <c r="AY7" t="n">
-        <v>1.406851172173316</v>
+        <v>1.070430239697088</v>
       </c>
       <c r="AZ7" t="n">
-        <v>1.067294015516125</v>
+        <v>58.93902494827333</v>
       </c>
       <c r="BA7" t="n">
-        <v>51.38520453833408</v>
+        <v>0.2038251421739935</v>
       </c>
       <c r="BB7" t="n">
-        <v>0.2200077900099006</v>
+        <v>0.1651014980682993</v>
       </c>
       <c r="BC7" t="n">
-        <v>0.1640501230299282</v>
+        <v>1.001371442545799</v>
       </c>
       <c r="BD7" t="n">
-        <v>0.9969977713715754</v>
+        <v>10.40074292691192</v>
       </c>
       <c r="BE7" t="n">
-        <v>11.86450259682727</v>
+        <v>4.542267856576755</v>
       </c>
       <c r="BF7" t="n">
-        <v>3.338327085063712</v>
+        <v>0.141880058524881</v>
       </c>
       <c r="BG7" t="n">
-        <v>0.8148074320626776</v>
+        <v>0.1018096561524466</v>
       </c>
       <c r="BH7" t="n">
-        <v>0.08780886754922472</v>
+        <v>0.4245393593432797</v>
       </c>
       <c r="BI7" t="n">
-        <v>0.4279451178499321</v>
+        <v>0</v>
       </c>
       <c r="BJ7" t="n">
-        <v>0.04972573964332937</v>
+        <v>0.0188886120982039</v>
       </c>
       <c r="BK7" t="n">
-        <v>0.01886664325310534</v>
+        <v>98.97724813334466</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>12.04269500735131</v>
       </c>
     </row>
     <row r="8">
@@ -2123,82 +2148,85 @@
         <v>0.3278336781347531</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.8257889543262364</v>
+        <v>1.441817750767649</v>
       </c>
       <c r="AM8" t="n">
-        <v>1.21940763169362</v>
+        <v>27.50931135157485</v>
       </c>
       <c r="AN8" t="n">
-        <v>36.17200757557804</v>
+        <v>0.6410695619587676</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.602459883197518</v>
+        <v>0.2108609591191313</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.2001921220729141</v>
+        <v>2.761270649281573</v>
       </c>
       <c r="AQ8" t="n">
-        <v>2.867910212374412</v>
+        <v>1757.448549785391</v>
       </c>
       <c r="AR8" t="n">
-        <v>1975.180402340506</v>
+        <v>8773.139319466225</v>
       </c>
       <c r="AS8" t="n">
-        <v>8256.659707941286</v>
+        <v>0.5236339236390973</v>
       </c>
       <c r="AT8" t="n">
-        <v>0.5776822246629038</v>
+        <v>0.3895320354834685</v>
       </c>
       <c r="AU8" t="n">
-        <v>0.3781134959642132</v>
+        <v>0.6418718672681835</v>
       </c>
       <c r="AV8" t="n">
-        <v>0.6120577298497099</v>
+        <v>10.55271948016741</v>
       </c>
       <c r="AW8" t="n">
-        <v>10.26688925218267</v>
+        <v>1.03695581447045</v>
       </c>
       <c r="AX8" t="n">
-        <v>0.9530600230690955</v>
+        <v>1.302200823599358</v>
       </c>
       <c r="AY8" t="n">
-        <v>1.197204441939972</v>
+        <v>0.9109164232151959</v>
       </c>
       <c r="AZ8" t="n">
-        <v>0.9522386467430114</v>
+        <v>52.58533875499692</v>
       </c>
       <c r="BA8" t="n">
-        <v>60.90168190963777</v>
+        <v>0.2415733105549236</v>
       </c>
       <c r="BB8" t="n">
-        <v>0.2448317706112908</v>
+        <v>0.183730276554386</v>
       </c>
       <c r="BC8" t="n">
-        <v>0.1765413259643002</v>
+        <v>1.034584075830855</v>
       </c>
       <c r="BD8" t="n">
-        <v>1.022939036191897</v>
+        <v>11.00505624591649</v>
       </c>
       <c r="BE8" t="n">
-        <v>11.4227674717584</v>
+        <v>4.25809690810217</v>
       </c>
       <c r="BF8" t="n">
-        <v>3.643653764995643</v>
+        <v>0.3498211776774951</v>
       </c>
       <c r="BG8" t="n">
-        <v>0.3934732072930236</v>
+        <v>0.08556863812620033</v>
       </c>
       <c r="BH8" t="n">
-        <v>0.09937162184255323</v>
+        <v>0.4754718941337104</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.3909656283116149</v>
+        <v>0</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0.03707059915965655</v>
+        <v>0.01725641393927127</v>
       </c>
       <c r="BK8" t="n">
-        <v>0.01757632030277021</v>
+        <v>75.85215387230998</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>11.29058407731956</v>
       </c>
     </row>
     <row r="9">
@@ -2314,82 +2342,85 @@
         <v>0.4000488166207219</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.8718056223439828</v>
+        <v>1.547840153880537</v>
       </c>
       <c r="AM9" t="n">
-        <v>1.693978440004883</v>
+        <v>38.21542453709838</v>
       </c>
       <c r="AN9" t="n">
-        <v>37.75858704724537</v>
+        <v>0.6679078532527447</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.5615157834396334</v>
+        <v>0.1965305242038717</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.2166309046691252</v>
+        <v>2.98801247819483</v>
       </c>
       <c r="AQ9" t="n">
-        <v>3.066981262011295</v>
+        <v>1879.438815024184</v>
       </c>
       <c r="AR9" t="n">
-        <v>1571.889312627439</v>
+        <v>6981.845262397033</v>
       </c>
       <c r="AS9" t="n">
-        <v>8194.520383700405</v>
+        <v>0.5196930735477172</v>
       </c>
       <c r="AT9" t="n">
-        <v>0.5248192209068461</v>
+        <v>0.3647370888905667</v>
       </c>
       <c r="AU9" t="n">
-        <v>0.3346616617857832</v>
+        <v>0.5282882503514874</v>
       </c>
       <c r="AV9" t="n">
-        <v>0.6642693064297771</v>
+        <v>11.45291907637547</v>
       </c>
       <c r="AW9" t="n">
-        <v>8.954694783856556</v>
+        <v>0.9044241731695122</v>
       </c>
       <c r="AX9" t="n">
-        <v>0.9792634401004914</v>
+        <v>1.338003512216513</v>
       </c>
       <c r="AY9" t="n">
-        <v>1.349007945617031</v>
+        <v>1.026419089056437</v>
       </c>
       <c r="AZ9" t="n">
-        <v>1.107992543784342</v>
+        <v>61.18651396075359</v>
       </c>
       <c r="BA9" t="n">
-        <v>60.49402496848921</v>
+        <v>0.239956293852658</v>
       </c>
       <c r="BB9" t="n">
-        <v>0.1984913140656065</v>
+        <v>0.1489547861205378</v>
       </c>
       <c r="BC9" t="n">
-        <v>0.1721178600286584</v>
+        <v>1.023543306229923</v>
       </c>
       <c r="BD9" t="n">
-        <v>1.048665088175501</v>
+        <v>11.80173547336474</v>
       </c>
       <c r="BE9" t="n">
-        <v>11.60695046537014</v>
+        <v>4.376582971394909</v>
       </c>
       <c r="BF9" t="n">
-        <v>3.768735645449274</v>
+        <v>0.4306228749602797</v>
       </c>
       <c r="BG9" t="n">
-        <v>0.6467689210439072</v>
+        <v>0.09422009163112199</v>
       </c>
       <c r="BH9" t="n">
-        <v>0.0827477427775748</v>
+        <v>0.3865877097643577</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.4624056191445205</v>
+        <v>0</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.04584529543694964</v>
+        <v>0.02040962732775814</v>
       </c>
       <c r="BK9" t="n">
-        <v>0.01793991031573964</v>
+        <v>92.16000256369774</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>11.5023059483976</v>
       </c>
     </row>
     <row r="10">
@@ -2505,82 +2536,85 @@
         <v>0.356986234738404</v>
       </c>
       <c r="AL10" t="n">
-        <v>0.9009311017585331</v>
+        <v>1.61494525845166</v>
       </c>
       <c r="AM10" t="n">
-        <v>1.190184398201379</v>
+        <v>26.8500477813434</v>
       </c>
       <c r="AN10" t="n">
-        <v>36.85207590298437</v>
+        <v>0.6512777935385762</v>
       </c>
       <c r="AO10" t="n">
-        <v>0.508177145720317</v>
+        <v>0.177862001002111</v>
       </c>
       <c r="AP10" t="n">
-        <v>0.2049085943199403</v>
+        <v>2.826325438895728</v>
       </c>
       <c r="AQ10" t="n">
-        <v>2.687351458956608</v>
+        <v>1646.802575592755</v>
       </c>
       <c r="AR10" t="n">
-        <v>1857.464137229572</v>
+        <v>8250.280145305887</v>
       </c>
       <c r="AS10" t="n">
-        <v>7332.994479529619</v>
+        <v>0.4650554591279565</v>
       </c>
       <c r="AT10" t="n">
-        <v>0.5087493067318933</v>
+        <v>0.3571996310200458</v>
       </c>
       <c r="AU10" t="n">
-        <v>0.3557827084903504</v>
+        <v>0.5866449645881191</v>
       </c>
       <c r="AV10" t="n">
-        <v>0.5532299908873968</v>
+        <v>9.538448118748221</v>
       </c>
       <c r="AW10" t="n">
-        <v>9.655707193063163</v>
+        <v>0.9752264264993795</v>
       </c>
       <c r="AX10" t="n">
-        <v>0.9233245121109723</v>
+        <v>1.261572105656576</v>
       </c>
       <c r="AY10" t="n">
-        <v>1.466587592660637</v>
+        <v>1.11588186398092</v>
       </c>
       <c r="AZ10" t="n">
-        <v>1.075310585553985</v>
+        <v>59.38172285024977</v>
       </c>
       <c r="BA10" t="n">
-        <v>57.25386526749773</v>
+        <v>0.227103839188819</v>
       </c>
       <c r="BB10" t="n">
-        <v>0.2057060123115453</v>
+        <v>0.1543689466303162</v>
       </c>
       <c r="BC10" t="n">
-        <v>0.2011141350060965</v>
+        <v>1.071747300390987</v>
       </c>
       <c r="BD10" t="n">
-        <v>1.030040222268664</v>
+        <v>11.17744008537902</v>
       </c>
       <c r="BE10" t="n">
-        <v>9.478007841632301</v>
+        <v>3.362176761146378</v>
       </c>
       <c r="BF10" t="n">
-        <v>3.493163893036179</v>
+        <v>0.247330846981989</v>
       </c>
       <c r="BG10" t="n">
-        <v>0.6976529418614186</v>
+        <v>0.09651830027839924</v>
       </c>
       <c r="BH10" t="n">
-        <v>0.09253358656816799</v>
+        <v>0.4460190283171462</v>
       </c>
       <c r="BI10" t="n">
-        <v>0.4802189659153601</v>
+        <v>0</v>
       </c>
       <c r="BJ10" t="n">
-        <v>0.04774858988941312</v>
+        <v>0.02119587159902278</v>
       </c>
       <c r="BK10" t="n">
-        <v>0.0207741558610088</v>
+        <v>95.5037500791131</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>13.38404434021309</v>
       </c>
     </row>
     <row r="11">
@@ -2696,82 +2730,85 @@
         <v>0.3662682925801036</v>
       </c>
       <c r="AL11" t="n">
-        <v>0.803874898150717</v>
+        <v>1.391327765339252</v>
       </c>
       <c r="AM11" t="n">
-        <v>1.40826925661936</v>
+        <v>31.76994832596433</v>
       </c>
       <c r="AN11" t="n">
-        <v>26.51481053516931</v>
+        <v>0.5141498958244761</v>
       </c>
       <c r="AO11" t="n">
-        <v>0.5798573082885774</v>
+        <v>0.2029500579010021</v>
       </c>
       <c r="AP11" t="n">
-        <v>0.193338052633226</v>
+        <v>2.666731760458289</v>
       </c>
       <c r="AQ11" t="n">
-        <v>3.225835291851658</v>
+        <v>1976.784186286478</v>
       </c>
       <c r="AR11" t="n">
-        <v>1812.925399751874</v>
+        <v>8052.452874165509</v>
       </c>
       <c r="AS11" t="n">
-        <v>7088.324256082953</v>
+        <v>0.4495385753477266</v>
       </c>
       <c r="AT11" t="n">
-        <v>0.4961087614677832</v>
+        <v>0.3513390987217835</v>
       </c>
       <c r="AU11" t="n">
-        <v>0.3508015811923019</v>
+        <v>0.5740338000473271</v>
       </c>
       <c r="AV11" t="n">
-        <v>0.6006270477016364</v>
+        <v>10.35563875347649</v>
       </c>
       <c r="AW11" t="n">
-        <v>8.554706684343547</v>
+        <v>0.8640253751186981</v>
       </c>
       <c r="AX11" t="n">
-        <v>1.013772704256978</v>
+        <v>1.385154784034286</v>
       </c>
       <c r="AY11" t="n">
-        <v>1.365910429649222</v>
+        <v>1.039279674733104</v>
       </c>
       <c r="AZ11" t="n">
-        <v>0.8823904587475233</v>
+        <v>48.72812224763465</v>
       </c>
       <c r="BA11" t="n">
-        <v>66.55198789721391</v>
+        <v>0.2639858791452677</v>
       </c>
       <c r="BB11" t="n">
-        <v>0.2551590523846143</v>
+        <v>0.1914802280068888</v>
       </c>
       <c r="BC11" t="n">
-        <v>0.1735068686802589</v>
+        <v>1.027296779714829</v>
       </c>
       <c r="BD11" t="n">
-        <v>1.034114744364202</v>
+        <v>11.28879782531936</v>
       </c>
       <c r="BE11" t="n">
-        <v>10.78804467704385</v>
+        <v>3.867735155650715</v>
       </c>
       <c r="BF11" t="n">
-        <v>4.776947844800086</v>
+        <v>0.7914296007817012</v>
       </c>
       <c r="BG11" t="n">
-        <v>0.4974984846938528</v>
+        <v>0.08827929218944659</v>
       </c>
       <c r="BH11" t="n">
-        <v>0.0855283882130532</v>
+        <v>0.4102041907259453</v>
       </c>
       <c r="BI11" t="n">
-        <v>0.4207772940304219</v>
+        <v>0</v>
       </c>
       <c r="BJ11" t="n">
-        <v>0.04197534673977287</v>
+        <v>0.01857223918479103</v>
       </c>
       <c r="BK11" t="n">
-        <v>0.01856405534077486</v>
+        <v>85.36119572420895</v>
+      </c>
+      <c r="BL11" t="n">
+        <v>11.86575144417808</v>
       </c>
     </row>
     <row r="12">
@@ -2887,82 +2924,85 @@
         <v>0.3464435473875559</v>
       </c>
       <c r="AL12" t="n">
-        <v>0.7341084061596351</v>
+        <v>1.230585767791799</v>
       </c>
       <c r="AM12" t="n">
-        <v>1.477904402437255</v>
+        <v>33.34088724542656</v>
       </c>
       <c r="AN12" t="n">
-        <v>33.67087600522575</v>
+        <v>0.6114946643780015</v>
       </c>
       <c r="AO12" t="n">
-        <v>0.5511216961606353</v>
+        <v>0.1928925936562224</v>
       </c>
       <c r="AP12" t="n">
-        <v>0.2059547341668781</v>
+        <v>2.840754954025904</v>
       </c>
       <c r="AQ12" t="n">
-        <v>2.959149872662247</v>
+        <v>1813.359996372491</v>
       </c>
       <c r="AR12" t="n">
-        <v>1698.103571834735</v>
+        <v>7542.449893152141</v>
       </c>
       <c r="AS12" t="n">
-        <v>8826.466359573385</v>
+        <v>0.5597708244275359</v>
       </c>
       <c r="AT12" t="n">
-        <v>0.5205612900670002</v>
+        <v>0.3627399422990216</v>
       </c>
       <c r="AU12" t="n">
-        <v>0.3442625846596739</v>
+        <v>0.5555248466415805</v>
       </c>
       <c r="AV12" t="n">
-        <v>0.5892601633889232</v>
+        <v>10.15965798946419</v>
       </c>
       <c r="AW12" t="n">
-        <v>10.78627145366162</v>
+        <v>1.089413416819823</v>
       </c>
       <c r="AX12" t="n">
-        <v>1.031934326248048</v>
+        <v>1.409969673487432</v>
       </c>
       <c r="AY12" t="n">
-        <v>1.502966309285909</v>
+        <v>1.143561322282757</v>
       </c>
       <c r="AZ12" t="n">
-        <v>0.9746303645151118</v>
+        <v>53.82187338670879</v>
       </c>
       <c r="BA12" t="n">
-        <v>55.01952820856599</v>
+        <v>0.2182410921628411</v>
       </c>
       <c r="BB12" t="n">
-        <v>0.2187086387308984</v>
+        <v>0.1641265697606655</v>
       </c>
       <c r="BC12" t="n">
-        <v>0.1810210677081927</v>
+        <v>1.043381927829895</v>
       </c>
       <c r="BD12" t="n">
-        <v>1.067656330279448</v>
+        <v>12.68489743124014</v>
       </c>
       <c r="BE12" t="n">
-        <v>12.75889667332667</v>
+        <v>5.117637118845081</v>
       </c>
       <c r="BF12" t="n">
-        <v>5.364680790255341</v>
+        <v>0.9763075083580499</v>
       </c>
       <c r="BG12" t="n">
-        <v>0.04580803761635215</v>
+        <v>0.07917383867261189</v>
       </c>
       <c r="BH12" t="n">
-        <v>0.09687913922080724</v>
+        <v>0.4647362437220499</v>
       </c>
       <c r="BI12" t="n">
-        <v>0.4375759541968932</v>
+        <v>0</v>
       </c>
       <c r="BJ12" t="n">
-        <v>0.04129343791784662</v>
+        <v>0.01931369728869046</v>
       </c>
       <c r="BK12" t="n">
-        <v>0.01618531276835956</v>
+        <v>84.13420755807149</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>10.48058735748711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enable fixed parameter uncertainty analysis
</commit_message>
<xml_diff>
--- a/CCU/EtOH/analyses/parameter_distributions/10_full_samples.xlsx
+++ b/CCU/EtOH/analyses/parameter_distributions/10_full_samples.xlsx
@@ -1070,193 +1070,193 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>73032.97970604681</v>
+        <v>79902.64637126429</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1925204102288536</v>
+        <v>0.2013360118123529</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3670407285669111</v>
+        <v>0.3814607333037985</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2043057118393568</v>
+        <v>0.2025827637054539</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2019072514227982</v>
+        <v>0.2005595593938897</v>
       </c>
       <c r="G3" t="n">
-        <v>0.03927911202641908</v>
+        <v>0.04090957294340732</v>
       </c>
       <c r="H3" t="n">
-        <v>353.4830521565772</v>
+        <v>316.5501262434337</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2606469573274428</v>
+        <v>0.1831451459710269</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1053262520424772</v>
+        <v>0.09772007024915925</v>
       </c>
       <c r="K3" t="n">
-        <v>0.08400681490809124</v>
+        <v>0.08584263690551329</v>
       </c>
       <c r="L3" t="n">
-        <v>0.126753825519268</v>
+        <v>0.1423540547076315</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8614635696451921</v>
+        <v>0.7164482504641035</v>
       </c>
       <c r="N3" t="n">
-        <v>0.4832990036692792</v>
+        <v>0.4844019663713621</v>
       </c>
       <c r="O3" t="n">
-        <v>0.08255568198683824</v>
+        <v>0.1165121922081832</v>
       </c>
       <c r="P3" t="n">
-        <v>1.377112554706376</v>
+        <v>1.272922751011066</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.8319373136991755</v>
+        <v>0.9575936016744718</v>
       </c>
       <c r="R3" t="n">
-        <v>0.8237218838231926</v>
+        <v>1.092509624454004</v>
       </c>
       <c r="S3" t="n">
-        <v>2.427954693056107</v>
+        <v>2.107487725683853</v>
       </c>
       <c r="T3" t="n">
-        <v>0.1190713997931622</v>
+        <v>0.1514522704342633</v>
       </c>
       <c r="U3" t="n">
-        <v>3.745131274119514</v>
+        <v>3.085131310701592</v>
       </c>
       <c r="V3" t="n">
-        <v>0.0009790382232347608</v>
+        <v>0.001144705756452408</v>
       </c>
       <c r="W3" t="n">
-        <v>0.00220367092654493</v>
+        <v>0.001893027537826718</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.05949348046052582</v>
+        <v>-0.05130295724434283</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.228777747051153</v>
+        <v>0.2061455695635404</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.02047432001477791</v>
+        <v>0.01907568677781881</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.09772841272037269</v>
+        <v>0.09183951272671667</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.7891203295069594</v>
+        <v>0.890587376739564</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.9609385323019222</v>
+        <v>0.9349131270270357</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.8408417148297029</v>
+        <v>0.856477512184266</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.8093781184622127</v>
+        <v>0.7996287746683847</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.7715911141863642</v>
+        <v>0.8194244634040068</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.792481427730481</v>
+        <v>0.7607483302969841</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.8604811245662413</v>
+        <v>0.7703512758969591</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.1228055786965717</v>
+        <v>0.1061996589031982</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.2538820313829133</v>
+        <v>0.3200370880108877</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.3124138832473172</v>
+        <v>0.3190400952603097</v>
       </c>
       <c r="AL3" t="n">
-        <v>1.610441603120029</v>
+        <v>1.222963787293518</v>
       </c>
       <c r="AM3" t="n">
-        <v>35.05433310351172</v>
+        <v>38.12879733869499</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.5457425662086453</v>
+        <v>0.6650050781832835</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.2193847589371362</v>
+        <v>0.2463950785060476</v>
       </c>
       <c r="AP3" t="n">
-        <v>3.148470948021103</v>
+        <v>3.264631910692696</v>
       </c>
       <c r="AQ3" t="n">
-        <v>1775.97755265085</v>
+        <v>1702.256381125974</v>
       </c>
       <c r="AR3" t="n">
-        <v>7931.094889518778</v>
+        <v>7562.209078673357</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.5490411458812133</v>
+        <v>0.4481189962198877</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.37367340144707</v>
+        <v>0.3211418048968571</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.4902450518123029</v>
+        <v>0.5418930767740915</v>
       </c>
       <c r="AV3" t="n">
-        <v>10.77160751421775</v>
+        <v>9.785242374807554</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.9894401171503726</v>
+        <v>1.018594099481779</v>
       </c>
       <c r="AX3" t="n">
-        <v>1.490153018184499</v>
+        <v>1.405614799050018</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.9385931689219965</v>
+        <v>0.9209754422595533</v>
       </c>
       <c r="AZ3" t="n">
-        <v>56.57737896924907</v>
+        <v>52.04709529616716</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.2501250524832314</v>
+        <v>0.262905020748714</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.1986943096418544</v>
+        <v>0.1716811711767653</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.9724759901946821</v>
+        <v>1.022614171450431</v>
       </c>
       <c r="BD3" t="n">
-        <v>12.0146966066097</v>
+        <v>11.62927873161609</v>
       </c>
       <c r="BE3" t="n">
-        <v>3.695731094996853</v>
+        <v>3.686574218561883</v>
       </c>
       <c r="BF3" t="n">
-        <v>0.6627996661674525</v>
+        <v>0.3232757311475846</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.08294154046556321</v>
+        <v>0.08361523332164308</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.4839756722869181</v>
+        <v>0.4323179946841607</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.02164267887190791</v>
+        <v>0.02145875543115607</v>
       </c>
       <c r="BK3" t="n">
-        <v>74.07127953482455</v>
+        <v>89.97124436466795</v>
       </c>
       <c r="BL3" t="n">
-        <v>12.8647189938306</v>
+        <v>11.13464757037698</v>
       </c>
     </row>
     <row r="4">
@@ -1264,193 +1264,193 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>87803.04413608434</v>
+        <v>96027.21121228262</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2246568959019964</v>
+        <v>0.1791255690542708</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3748139406789477</v>
+        <v>0.3726661441021397</v>
       </c>
       <c r="E4" t="n">
-        <v>0.206092812456228</v>
+        <v>0.2080152351211102</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2050068609135489</v>
+        <v>0.2084664638077784</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05274573767178555</v>
+        <v>0.04652838658780319</v>
       </c>
       <c r="H4" t="n">
-        <v>302.8640470471933</v>
+        <v>329.5918150567987</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2457587789998857</v>
+        <v>0.2481632847540977</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1035825605074916</v>
+        <v>0.09371249497774604</v>
       </c>
       <c r="K4" t="n">
-        <v>0.09002969327840353</v>
+        <v>0.08817987563675377</v>
       </c>
       <c r="L4" t="n">
-        <v>0.148656010476794</v>
+        <v>0.1608026425684443</v>
       </c>
       <c r="M4" t="n">
-        <v>0.7419830689790785</v>
+        <v>0.9012489559240373</v>
       </c>
       <c r="N4" t="n">
-        <v>0.388489729370968</v>
+        <v>0.3557525486739259</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1116319649202889</v>
+        <v>0.08509887361978358</v>
       </c>
       <c r="P4" t="n">
-        <v>1.204052509079161</v>
+        <v>1.167552929012193</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.9879764702657847</v>
+        <v>0.8831952362740134</v>
       </c>
       <c r="R4" t="n">
-        <v>1.096422766431794</v>
+        <v>0.8286969511651712</v>
       </c>
       <c r="S4" t="n">
-        <v>2.158093885003253</v>
+        <v>2.024355681409083</v>
       </c>
       <c r="T4" t="n">
-        <v>0.1236120530717648</v>
+        <v>0.1393036501417461</v>
       </c>
       <c r="U4" t="n">
-        <v>2.909796470944358</v>
+        <v>3.567576488694518</v>
       </c>
       <c r="V4" t="n">
-        <v>0.001013542572170135</v>
+        <v>0.0009911801291056027</v>
       </c>
       <c r="W4" t="n">
-        <v>0.00249337234393538</v>
+        <v>0.002271083592123357</v>
       </c>
       <c r="X4" t="n">
-        <v>-0.05625959840710235</v>
+        <v>-0.05368721279917646</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.2192447650747515</v>
+        <v>0.1948887642174865</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.01749953088140552</v>
+        <v>0.02087377939516183</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.1069853913315458</v>
+        <v>0.0980348629145094</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.8549819810532457</v>
+        <v>0.8573712054361631</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.9510431959459896</v>
+        <v>0.9223631997900019</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.8581837226391104</v>
+        <v>0.8422412167846233</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.8851662867134981</v>
+        <v>0.847852894684107</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.7926186049176994</v>
+        <v>0.8148386549742012</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.8022658412554833</v>
+        <v>0.8168930657682468</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.8884298290543484</v>
+        <v>0.8654323778489769</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.1118644972717975</v>
+        <v>0.1106755761690634</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.2994595586986581</v>
+        <v>0.2989588798737637</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.3304005894647825</v>
+        <v>0.3575438435396859</v>
       </c>
       <c r="AL4" t="n">
-        <v>1.374653351742964</v>
+        <v>1.694906019601306</v>
       </c>
       <c r="AM4" t="n">
-        <v>28.99971444356492</v>
+        <v>35.82083235711326</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.6160891480559249</v>
+        <v>0.5319955920135586</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.2228202252306173</v>
+        <v>0.1934947933822437</v>
       </c>
       <c r="AP4" t="n">
-        <v>2.566982632055544</v>
+        <v>2.94548072863882</v>
       </c>
       <c r="AQ4" t="n">
-        <v>1937.613448346334</v>
+        <v>1625.296586768909</v>
       </c>
       <c r="AR4" t="n">
-        <v>7030.599125762525</v>
+        <v>7832.801459048003</v>
       </c>
       <c r="AS4" t="n">
-        <v>0.4935944628966716</v>
+        <v>0.4904413151962091</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.337227592694029</v>
+        <v>0.3469074992744503</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.6519916413437414</v>
+        <v>0.5785442403634359</v>
       </c>
       <c r="AV4" t="n">
-        <v>9.91086913666507</v>
+        <v>10.62513639848103</v>
       </c>
       <c r="AW4" t="n">
-        <v>1.072590836245457</v>
+        <v>0.9289392130559706</v>
       </c>
       <c r="AX4" t="n">
-        <v>1.198103686556453</v>
+        <v>1.51218896955732</v>
       </c>
       <c r="AY4" t="n">
-        <v>1.166393347129673</v>
+        <v>1.031206256542402</v>
       </c>
       <c r="AZ4" t="n">
-        <v>57.46967160894422</v>
+        <v>58.79428159344904</v>
       </c>
       <c r="BA4" t="n">
-        <v>0.2318133471085047</v>
+        <v>0.243202018490852</v>
       </c>
       <c r="BB4" t="n">
-        <v>0.1735871823059199</v>
+        <v>0.1769989859973291</v>
       </c>
       <c r="BC4" t="n">
-        <v>1.008739037829258</v>
+        <v>0.9924120033586177</v>
       </c>
       <c r="BD4" t="n">
-        <v>9.550657567064762</v>
+        <v>12.27036629471784</v>
       </c>
       <c r="BE4" t="n">
-        <v>4.037414950784498</v>
+        <v>4.44194884746188</v>
       </c>
       <c r="BF4" t="n">
-        <v>0.5212509579126134</v>
+        <v>0.0485373691896562</v>
       </c>
       <c r="BG4" t="n">
-        <v>0.09968215604725696</v>
+        <v>0.08990329839236617</v>
       </c>
       <c r="BH4" t="n">
-        <v>0.3993009170013498</v>
+        <v>0.4920214678557828</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.01804378407058523</v>
+        <v>0.02023966536019519</v>
       </c>
       <c r="BK4" t="n">
-        <v>87.83610107529771</v>
+        <v>73.49088950860263</v>
       </c>
       <c r="BL4" t="n">
-        <v>13.95274385466979</v>
+        <v>13.83070451443536</v>
       </c>
     </row>
     <row r="5">
@@ -1458,193 +1458,193 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>82969.40355652415</v>
+        <v>82678.66997076318</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1823024282749421</v>
+        <v>0.1928299623188101</v>
       </c>
       <c r="D5" t="n">
-        <v>0.356156809543878</v>
+        <v>0.349514353677673</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2062168464084541</v>
+        <v>0.2046533437350419</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1930081485261441</v>
+        <v>0.201753395363712</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0376881032860245</v>
+        <v>0.03882999145642547</v>
       </c>
       <c r="H5" t="n">
-        <v>328.3938182107083</v>
+        <v>342.2810642110288</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1797874888071544</v>
+        <v>0.1655495029491964</v>
       </c>
       <c r="J5" t="n">
-        <v>0.09218373153518364</v>
+        <v>0.1078719783435765</v>
       </c>
       <c r="K5" t="n">
-        <v>0.09790202495792344</v>
+        <v>0.09381089769825053</v>
       </c>
       <c r="L5" t="n">
-        <v>0.13850123834134</v>
+        <v>0.118104483940798</v>
       </c>
       <c r="M5" t="n">
-        <v>1.039746259944121</v>
+        <v>0.9370256781547696</v>
       </c>
       <c r="N5" t="n">
-        <v>0.4151378366360204</v>
+        <v>0.4138128391637069</v>
       </c>
       <c r="O5" t="n">
-        <v>0.08454748544920931</v>
+        <v>0.08792587709614851</v>
       </c>
       <c r="P5" t="n">
-        <v>1.085036497613372</v>
+        <v>1.299389456365677</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.7684202836069705</v>
+        <v>0.9160973244915677</v>
       </c>
       <c r="R5" t="n">
-        <v>0.8915111400973487</v>
+        <v>0.9682119235958253</v>
       </c>
       <c r="S5" t="n">
-        <v>1.932709456420227</v>
+        <v>2.18465134980983</v>
       </c>
       <c r="T5" t="n">
-        <v>0.1359759237173337</v>
+        <v>0.1379768838876931</v>
       </c>
       <c r="U5" t="n">
-        <v>3.513905511143649</v>
+        <v>3.263158588752137</v>
       </c>
       <c r="V5" t="n">
-        <v>0.0009683448509377951</v>
+        <v>0.001092568104502902</v>
       </c>
       <c r="W5" t="n">
-        <v>0.001962172038385517</v>
+        <v>0.002569023462270782</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.05042028557202284</v>
+        <v>-0.0597926796920753</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.2147480623904435</v>
+        <v>0.1811251643771146</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.02674240147582884</v>
+        <v>0.02558203428032398</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.09961480269475323</v>
+        <v>0.09504726960594857</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.8877916071006047</v>
+        <v>0.9070870689343291</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.9486768942663376</v>
+        <v>0.9115238014528035</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.8379363122779646</v>
+        <v>0.8380090792918973</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.8611389585077722</v>
+        <v>0.9434523997721935</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.8083644183139171</v>
+        <v>0.7746676947465968</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.7713592057814963</v>
+        <v>0.8393851853614266</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.8139179200758813</v>
+        <v>0.9306427050528593</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.1079511876231142</v>
+        <v>0.114683287953233</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.3110956311139123</v>
+        <v>0.2495719450656144</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.3478657624522924</v>
+        <v>0.3478206052239455</v>
       </c>
       <c r="AL5" t="n">
-        <v>1.314768028390332</v>
+        <v>1.521434043633305</v>
       </c>
       <c r="AM5" t="n">
-        <v>35.59609622838455</v>
+        <v>31.37906514834588</v>
       </c>
       <c r="AN5" t="n">
-        <v>0.5744787627083249</v>
+        <v>0.5912194440582774</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.2087577315703888</v>
+        <v>0.2231728277025448</v>
       </c>
       <c r="AP5" t="n">
-        <v>2.936544603381268</v>
+        <v>3.057329622170576</v>
       </c>
       <c r="AQ5" t="n">
-        <v>1589.725707208001</v>
+        <v>1786.685871696152</v>
       </c>
       <c r="AR5" t="n">
-        <v>7491.199990571404</v>
+        <v>7220.681163563626</v>
       </c>
       <c r="AS5" t="n">
-        <v>0.5008703037403166</v>
+        <v>0.5281607572940125</v>
       </c>
       <c r="AT5" t="n">
-        <v>0.3416436480382924</v>
+        <v>0.3434381097779279</v>
       </c>
       <c r="AU5" t="n">
-        <v>0.6105354633924327</v>
+        <v>0.58704840593991</v>
       </c>
       <c r="AV5" t="n">
-        <v>8.908075913142451</v>
+        <v>10.27734818577751</v>
       </c>
       <c r="AW5" t="n">
-        <v>1.122056117300043</v>
+        <v>0.9675875580093848</v>
       </c>
       <c r="AX5" t="n">
-        <v>1.364631501937441</v>
+        <v>1.284282369798197</v>
       </c>
       <c r="AY5" t="n">
-        <v>1.092516857922506</v>
+        <v>1.101757730440204</v>
       </c>
       <c r="AZ5" t="n">
-        <v>63.09528618653049</v>
+        <v>54.64124469425514</v>
       </c>
       <c r="BA5" t="n">
-        <v>0.2093884387428838</v>
+        <v>0.2293489904915698</v>
       </c>
       <c r="BB5" t="n">
-        <v>0.1714062109570489</v>
+        <v>0.1616944278292475</v>
       </c>
       <c r="BC5" t="n">
-        <v>1.05125004502594</v>
+        <v>0.9828511478953185</v>
       </c>
       <c r="BD5" t="n">
-        <v>10.56167962869034</v>
+        <v>10.50355596857512</v>
       </c>
       <c r="BE5" t="n">
-        <v>3.962748497191042</v>
+        <v>3.422763698065878</v>
       </c>
       <c r="BF5" t="n">
-        <v>0.5562972997006265</v>
+        <v>0.5704003225521048</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.09078781509376259</v>
+        <v>0.1087888903588528</v>
       </c>
       <c r="BH5" t="n">
-        <v>0.4386314325985388</v>
+        <v>0.4817351634151865</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="BJ5" t="n">
-        <v>0.01981402385718399</v>
+        <v>0.01911439164946262</v>
       </c>
       <c r="BK5" t="n">
-        <v>62.15276524669687</v>
+        <v>81.4722705298153</v>
       </c>
       <c r="BL5" t="n">
-        <v>13.03500049392157</v>
+        <v>12.83584642459542</v>
       </c>
     </row>
     <row r="6">
@@ -1652,193 +1652,193 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>92990.56979982168</v>
+        <v>69195.06094623517</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2046054600480584</v>
+        <v>0.2335232139983855</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3632209997453922</v>
+        <v>0.3556125383902581</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2086000458092738</v>
+        <v>0.202159870171003</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1982608378620102</v>
+        <v>0.1937619101610563</v>
       </c>
       <c r="G6" t="n">
-        <v>0.04979524876199633</v>
+        <v>0.05186755277070323</v>
       </c>
       <c r="H6" t="n">
-        <v>342.053369907208</v>
+        <v>304.2925834996341</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1539233253859425</v>
+        <v>0.1576728156318847</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1099292083761779</v>
+        <v>0.1159992474279312</v>
       </c>
       <c r="K6" t="n">
-        <v>0.08670084948586733</v>
+        <v>0.09175560370974323</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1576670693616104</v>
+        <v>0.127958906170922</v>
       </c>
       <c r="M6" t="n">
-        <v>1.00085621773082</v>
+        <v>1.017425150534883</v>
       </c>
       <c r="N6" t="n">
-        <v>0.4269877242588999</v>
+        <v>0.3911001010850896</v>
       </c>
       <c r="O6" t="n">
-        <v>0.1006303632643175</v>
+        <v>0.09384800242706398</v>
       </c>
       <c r="P6" t="n">
-        <v>1.165122768271854</v>
+        <v>1.118394927587925</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.025412481489324</v>
+        <v>1.028547596444965</v>
       </c>
       <c r="R6" t="n">
-        <v>1.038717275160321</v>
+        <v>0.7986213135815405</v>
       </c>
       <c r="S6" t="n">
-        <v>2.079257940521597</v>
+        <v>2.438365084609514</v>
       </c>
       <c r="T6" t="n">
-        <v>0.1404866864370876</v>
+        <v>0.1197155506340309</v>
       </c>
       <c r="U6" t="n">
-        <v>3.901243295520608</v>
+        <v>3.486008802446065</v>
       </c>
       <c r="V6" t="n">
-        <v>0.00117866902771296</v>
+        <v>0.000970646815018182</v>
       </c>
       <c r="W6" t="n">
-        <v>0.00214208049788564</v>
+        <v>0.002432968111207338</v>
       </c>
       <c r="X6" t="n">
-        <v>-0.05529398728184307</v>
+        <v>-0.05907352604414596</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.2048323254635424</v>
+        <v>0.2270330940715378</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.01819726907556523</v>
+        <v>0.01684217765784487</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.1042423041895399</v>
+        <v>0.102783290049627</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.9019201562515629</v>
+        <v>0.8222316380124366</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.9320951239522288</v>
+        <v>0.9403644023351871</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.8614816440750417</v>
+        <v>0.865590443750378</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.7908688486417349</v>
+        <v>0.8317460289926938</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.7854195592499511</v>
+        <v>0.8025902468005439</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.7217601269939683</v>
+        <v>0.8752336086261902</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.839540680647087</v>
+        <v>0.8418818383535213</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.1191888842079433</v>
+        <v>0.100436000991509</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.277339701620288</v>
+        <v>0.2920120871299834</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.3898367736965631</v>
+        <v>0.3665693293758379</v>
       </c>
       <c r="AL6" t="n">
-        <v>1.179703414151158</v>
+        <v>1.446607923705237</v>
       </c>
       <c r="AM6" t="n">
-        <v>37.28116357119865</v>
+        <v>27.31610557634989</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.597935546608431</v>
+        <v>0.5397622087778048</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.2420829950158175</v>
+        <v>0.2095805311687465</v>
       </c>
       <c r="AP6" t="n">
-        <v>3.323935627024253</v>
+        <v>3.0207961791712</v>
       </c>
       <c r="AQ6" t="n">
-        <v>1703.945334520654</v>
+        <v>1675.529259288374</v>
       </c>
       <c r="AR6" t="n">
-        <v>8699.012502715061</v>
+        <v>9002.673359440871</v>
       </c>
       <c r="AS6" t="n">
-        <v>0.4825365945650992</v>
+        <v>0.5027557816687551</v>
       </c>
       <c r="AT6" t="n">
-        <v>0.3290039135592568</v>
+        <v>0.3516979672811477</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.6043096595951036</v>
+        <v>0.6538845857080131</v>
       </c>
       <c r="AV6" t="n">
-        <v>8.885982583338841</v>
+        <v>8.446441509554655</v>
       </c>
       <c r="AW6" t="n">
-        <v>1.013834558372801</v>
+        <v>0.8622173704949254</v>
       </c>
       <c r="AX6" t="n">
-        <v>1.581524420806664</v>
+        <v>1.567059351214774</v>
       </c>
       <c r="AY6" t="n">
-        <v>0.9966519745468041</v>
+        <v>1.167065819603704</v>
       </c>
       <c r="AZ6" t="n">
-        <v>65.95827346199394</v>
+        <v>56.47692083049123</v>
       </c>
       <c r="BA6" t="n">
-        <v>0.2199357829956745</v>
+        <v>0.251549736719905</v>
       </c>
       <c r="BB6" t="n">
-        <v>0.1789383324114011</v>
+        <v>0.1474553041668592</v>
       </c>
       <c r="BC6" t="n">
-        <v>0.9409126331199501</v>
+        <v>1.031029952905833</v>
       </c>
       <c r="BD6" t="n">
-        <v>10.01489573772551</v>
+        <v>11.42051729056949</v>
       </c>
       <c r="BE6" t="n">
-        <v>3.637120146400111</v>
+        <v>3.834840145865092</v>
       </c>
       <c r="BF6" t="n">
-        <v>0.6037424768687916</v>
+        <v>0.6154743051202975</v>
       </c>
       <c r="BG6" t="n">
-        <v>0.086653942166265</v>
+        <v>0.09449476423820384</v>
       </c>
       <c r="BH6" t="n">
-        <v>0.4333856775346247</v>
+        <v>0.4614138583536601</v>
       </c>
       <c r="BI6" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="BJ6" t="n">
-        <v>0.0156295127061641</v>
+        <v>0.01759507781665342</v>
       </c>
       <c r="BK6" t="n">
-        <v>81.73756212032436</v>
+        <v>64.23424538522323</v>
       </c>
       <c r="BL6" t="n">
-        <v>12.39181050235996</v>
+        <v>12.53913482515483</v>
       </c>
     </row>
     <row r="7">
@@ -1846,193 +1846,193 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>91927.32837790748</v>
+        <v>78353.19773949904</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1981344474449643</v>
+        <v>0.1765902128583643</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3773436737302281</v>
+        <v>0.391009740344253</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2002301973368371</v>
+        <v>0.2090840738095038</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2086730390173199</v>
+        <v>0.1966197102311658</v>
       </c>
       <c r="G7" t="n">
-        <v>0.04443218895052526</v>
+        <v>0.03791421958433679</v>
       </c>
       <c r="H7" t="n">
-        <v>331.9127824768815</v>
+        <v>338.9805970192066</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2230516606175751</v>
+        <v>0.261836193222695</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1190956415677746</v>
+        <v>0.08151105421631745</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0890391422247139</v>
+        <v>0.09703986269254358</v>
       </c>
       <c r="L7" t="n">
-        <v>0.165083673113302</v>
+        <v>0.1719610348754591</v>
       </c>
       <c r="M7" t="n">
-        <v>0.8308578047056688</v>
+        <v>0.8173218836892334</v>
       </c>
       <c r="N7" t="n">
-        <v>0.3573380834898047</v>
+        <v>0.4634179693947457</v>
       </c>
       <c r="O7" t="n">
-        <v>0.09588698025044802</v>
+        <v>0.08017915844392824</v>
       </c>
       <c r="P7" t="n">
-        <v>1.314932999204314</v>
+        <v>1.079721062531109</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.9803330312555119</v>
+        <v>0.7594465656405882</v>
       </c>
       <c r="R7" t="n">
-        <v>0.7709063241338732</v>
+        <v>0.8749555256208853</v>
       </c>
       <c r="S7" t="n">
-        <v>1.842475609561873</v>
+        <v>1.878739440753441</v>
       </c>
       <c r="T7" t="n">
-        <v>0.1278878260875293</v>
+        <v>0.1336113023247245</v>
       </c>
       <c r="U7" t="n">
-        <v>3.322507548641651</v>
+        <v>4.140236347423852</v>
       </c>
       <c r="V7" t="n">
-        <v>0.001113337927623731</v>
+        <v>0.001120113957685961</v>
       </c>
       <c r="W7" t="n">
-        <v>0.002091300166484687</v>
+        <v>0.002375586185025747</v>
       </c>
       <c r="X7" t="n">
-        <v>-0.0527005047583998</v>
+        <v>-0.0554020501558226</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.192869361017758</v>
+        <v>0.1906312758863251</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.01445613826704669</v>
+        <v>0.01886841466403571</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.09817969816050011</v>
+        <v>0.1021498835936329</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.8657712139417229</v>
+        <v>0.918006673395242</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.9239494565029579</v>
+        <v>0.9492287882550789</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.8759867831331991</v>
+        <v>0.8095708326318948</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.9147083127897548</v>
+        <v>0.8153862310332183</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.8329842428718318</v>
+        <v>0.8108444952810935</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.8560462070902725</v>
+        <v>0.8056480336527307</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.7972297299411926</v>
+        <v>0.8920566266636781</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.10679789534363</v>
+        <v>0.1079819898201331</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.3049403619051028</v>
+        <v>0.2578576620604025</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.3755015056236315</v>
+        <v>0.3721248230270345</v>
       </c>
       <c r="AL7" t="n">
-        <v>1.679416103783271</v>
+        <v>1.620799454411124</v>
       </c>
       <c r="AM7" t="n">
-        <v>30.90956824459912</v>
+        <v>32.68928228784205</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.556183449416613</v>
+        <v>0.622141038763919</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.2283334829752033</v>
+        <v>0.2050522458779884</v>
       </c>
       <c r="AP7" t="n">
-        <v>3.058268242296375</v>
+        <v>2.811269195668324</v>
       </c>
       <c r="AQ7" t="n">
-        <v>1560.941303704969</v>
+        <v>1906.354441648915</v>
       </c>
       <c r="AR7" t="n">
-        <v>7801.035503897236</v>
+        <v>7000.15421379756</v>
       </c>
       <c r="AS7" t="n">
-        <v>0.4352266946764374</v>
+        <v>0.4365038750145921</v>
       </c>
       <c r="AT7" t="n">
-        <v>0.345997014974413</v>
+        <v>0.3930868637215483</v>
       </c>
       <c r="AU7" t="n">
-        <v>0.5528954941372662</v>
+        <v>0.592717272542591</v>
       </c>
       <c r="AV7" t="n">
-        <v>9.780835343552964</v>
+        <v>9.065800255884469</v>
       </c>
       <c r="AW7" t="n">
-        <v>0.9457116738311282</v>
+        <v>1.080718226065067</v>
       </c>
       <c r="AX7" t="n">
-        <v>1.448966930156673</v>
+        <v>1.178656187717872</v>
       </c>
       <c r="AY7" t="n">
-        <v>1.070430239697088</v>
+        <v>1.051181330189068</v>
       </c>
       <c r="AZ7" t="n">
-        <v>58.93902494827333</v>
+        <v>51.42099187186224</v>
       </c>
       <c r="BA7" t="n">
-        <v>0.2038251421739935</v>
+        <v>0.196331215270054</v>
       </c>
       <c r="BB7" t="n">
-        <v>0.1651014980682993</v>
+        <v>0.1814914949845403</v>
       </c>
       <c r="BC7" t="n">
-        <v>1.001371442545799</v>
+        <v>1.046304324705986</v>
       </c>
       <c r="BD7" t="n">
-        <v>10.40074292691192</v>
+        <v>11.21146521299333</v>
       </c>
       <c r="BE7" t="n">
-        <v>4.542267856576755</v>
+        <v>5.163754579649339</v>
       </c>
       <c r="BF7" t="n">
-        <v>0.141880058524881</v>
+        <v>0.8696784273238116</v>
       </c>
       <c r="BG7" t="n">
-        <v>0.1018096561524466</v>
+        <v>0.08542961366878338</v>
       </c>
       <c r="BH7" t="n">
-        <v>0.4245393593432797</v>
+        <v>0.4400082855044671</v>
       </c>
       <c r="BI7" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="BJ7" t="n">
-        <v>0.0188886120982039</v>
+        <v>0.01873673367558694</v>
       </c>
       <c r="BK7" t="n">
-        <v>98.97724813334466</v>
+        <v>101.1373562088558</v>
       </c>
       <c r="BL7" t="n">
-        <v>12.04269500735131</v>
+        <v>13.03911891687778</v>
       </c>
     </row>
     <row r="8">
@@ -2040,193 +2040,193 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>81344.75003858029</v>
+        <v>89414.57688601717</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2000364141566252</v>
+        <v>0.2163269834227601</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3444469005496613</v>
+        <v>0.3502295841055854</v>
       </c>
       <c r="E8" t="n">
-        <v>0.202974238787211</v>
+        <v>0.2067574155604608</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2115095299545866</v>
+        <v>0.2124296338715219</v>
       </c>
       <c r="G8" t="n">
-        <v>0.04223074481359274</v>
+        <v>0.04209765564834488</v>
       </c>
       <c r="H8" t="n">
-        <v>336.1225938728379</v>
+        <v>336.6212099699324</v>
       </c>
       <c r="I8" t="n">
-        <v>0.229876204324823</v>
+        <v>0.235298596518741</v>
       </c>
       <c r="J8" t="n">
-        <v>0.08325004513040257</v>
+        <v>0.119694293059446</v>
       </c>
       <c r="K8" t="n">
-        <v>0.09178038316818182</v>
+        <v>0.1044345117871842</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1436228161719526</v>
+        <v>0.1306178533181063</v>
       </c>
       <c r="M8" t="n">
-        <v>0.7141994774516407</v>
+        <v>1.005101690769233</v>
       </c>
       <c r="N8" t="n">
-        <v>0.3746822830163015</v>
+        <v>0.44696800434708</v>
       </c>
       <c r="O8" t="n">
-        <v>0.1099620157713296</v>
+        <v>0.0971968666691601</v>
       </c>
       <c r="P8" t="n">
-        <v>1.2837617060289</v>
+        <v>0.9872153352176587</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.7342271884941617</v>
+        <v>0.7745752739143372</v>
       </c>
       <c r="R8" t="n">
-        <v>0.8789535293602975</v>
+        <v>0.7443963558086968</v>
       </c>
       <c r="S8" t="n">
-        <v>2.51003769048274</v>
+        <v>2.359234357949089</v>
       </c>
       <c r="T8" t="n">
-        <v>0.1330474537134463</v>
+        <v>0.128070814447214</v>
       </c>
       <c r="U8" t="n">
-        <v>3.472323208369935</v>
+        <v>3.781671274864095</v>
       </c>
       <c r="V8" t="n">
-        <v>0.001130389387685748</v>
+        <v>0.001231057321283688</v>
       </c>
       <c r="W8" t="n">
-        <v>0.002224477895711362</v>
+        <v>0.002249429899392879</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.05412418570081827</v>
+        <v>-0.05284230746120861</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.2098881469757531</v>
+        <v>0.2314598568521448</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.01969590737834712</v>
+        <v>0.02313129977383251</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.1016685840690763</v>
+        <v>0.1037415450808332</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.8056302072337234</v>
+        <v>0.8984338334851857</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.9572293750750147</v>
+        <v>0.9305634804949419</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.8524439236653476</v>
+        <v>0.8821192164064942</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.8405422131257322</v>
+        <v>0.8633687849188129</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.7810720067931854</v>
+        <v>0.7903683147213321</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.8338921029549079</v>
+        <v>0.7518708118296286</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.9196264233201109</v>
+        <v>0.8263880273109651</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.09569865480647581</v>
+        <v>0.1193769998309205</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.2725442640620873</v>
+        <v>0.3305043874258321</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.3278336781347531</v>
+        <v>0.3829416764470947</v>
       </c>
       <c r="AL8" t="n">
-        <v>1.441817750767649</v>
+        <v>1.187055718765812</v>
       </c>
       <c r="AM8" t="n">
-        <v>27.50931135157485</v>
+        <v>31.00620749219718</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.6410695619587676</v>
+        <v>0.5806010541292046</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.2108609591191313</v>
+        <v>0.1814968890923445</v>
       </c>
       <c r="AP8" t="n">
-        <v>2.761270649281573</v>
+        <v>2.74657995130602</v>
       </c>
       <c r="AQ8" t="n">
-        <v>1757.448549785391</v>
+        <v>1978.171403966057</v>
       </c>
       <c r="AR8" t="n">
-        <v>8773.139319466225</v>
+        <v>7498.90503107719</v>
       </c>
       <c r="AS8" t="n">
-        <v>0.5236339236390973</v>
+        <v>0.5528193058801828</v>
       </c>
       <c r="AT8" t="n">
-        <v>0.3895320354834685</v>
+        <v>0.373173962563687</v>
       </c>
       <c r="AU8" t="n">
-        <v>0.6418718672681835</v>
+        <v>0.5368910034635822</v>
       </c>
       <c r="AV8" t="n">
-        <v>10.55271948016741</v>
+        <v>11.00323726583764</v>
       </c>
       <c r="AW8" t="n">
-        <v>1.03695581447045</v>
+        <v>1.190590280662384</v>
       </c>
       <c r="AX8" t="n">
-        <v>1.302200823599358</v>
+        <v>1.42931381319706</v>
       </c>
       <c r="AY8" t="n">
-        <v>0.9109164232151959</v>
+        <v>1.128737793335133</v>
       </c>
       <c r="AZ8" t="n">
-        <v>52.58533875499692</v>
+        <v>57.80939853446883</v>
       </c>
       <c r="BA8" t="n">
-        <v>0.2415733105549236</v>
+        <v>0.2168215361075473</v>
       </c>
       <c r="BB8" t="n">
-        <v>0.183730276554386</v>
+        <v>0.2002548263837623</v>
       </c>
       <c r="BC8" t="n">
-        <v>1.034584075830855</v>
+        <v>1.010789783037349</v>
       </c>
       <c r="BD8" t="n">
-        <v>11.00505624591649</v>
+        <v>12.28547425956682</v>
       </c>
       <c r="BE8" t="n">
-        <v>4.25809690810217</v>
+        <v>4.129641247746418</v>
       </c>
       <c r="BF8" t="n">
-        <v>0.3498211776774951</v>
+        <v>0.4675084522349116</v>
       </c>
       <c r="BG8" t="n">
-        <v>0.08556863812620033</v>
+        <v>0.09489870194549964</v>
       </c>
       <c r="BH8" t="n">
-        <v>0.4754718941337104</v>
+        <v>0.4211453948106605</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0.01725641393927127</v>
+        <v>0.02128804584968809</v>
       </c>
       <c r="BK8" t="n">
-        <v>75.85215387230998</v>
+        <v>95.37794355856285</v>
       </c>
       <c r="BL8" t="n">
-        <v>11.29058407731956</v>
+        <v>10.89396261388824</v>
       </c>
     </row>
     <row r="9">
@@ -2234,193 +2234,193 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>86068.49414557515</v>
+        <v>84516.8554255318</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1867632897639113</v>
+        <v>0.186844555146999</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3535068242090964</v>
+        <v>0.3615377291323481</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2156715954870396</v>
+        <v>0.2116792508246128</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1965382702628646</v>
+        <v>0.1982853971300713</v>
       </c>
       <c r="G9" t="n">
-        <v>0.03502515086692526</v>
+        <v>0.05342401014756964</v>
       </c>
       <c r="H9" t="n">
-        <v>345.7356520247503</v>
+        <v>353.6451888955281</v>
       </c>
       <c r="I9" t="n">
-        <v>0.174201793551663</v>
+        <v>0.2799323772756739</v>
       </c>
       <c r="J9" t="n">
-        <v>0.09058053963673147</v>
+        <v>0.08934355683842228</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1037401421500932</v>
+        <v>0.0822062233570085</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1745563392340495</v>
+        <v>0.1465726670203443</v>
       </c>
       <c r="M9" t="n">
-        <v>0.9615629175881047</v>
+        <v>0.9527488271782349</v>
       </c>
       <c r="N9" t="n">
-        <v>0.4473047217822119</v>
+        <v>0.3959800550002982</v>
       </c>
       <c r="O9" t="n">
-        <v>0.1183876898348002</v>
+        <v>0.1001474907236696</v>
       </c>
       <c r="P9" t="n">
-        <v>1.109605248594028</v>
+        <v>1.201655707980408</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.8566784843135921</v>
+        <v>0.8388449947104305</v>
       </c>
       <c r="R9" t="n">
-        <v>0.7915588470506409</v>
+        <v>1.018406771890811</v>
       </c>
       <c r="S9" t="n">
-        <v>2.017660846661838</v>
+        <v>1.934319711586696</v>
       </c>
       <c r="T9" t="n">
-        <v>0.1448173331888827</v>
+        <v>0.1293835658566501</v>
       </c>
       <c r="U9" t="n">
-        <v>3.617868842415996</v>
+        <v>3.542595375886238</v>
       </c>
       <c r="V9" t="n">
-        <v>0.001143351635605225</v>
+        <v>0.001055818400199963</v>
       </c>
       <c r="W9" t="n">
-        <v>0.002340312955542357</v>
+        <v>0.002051627519851175</v>
       </c>
       <c r="X9" t="n">
-        <v>-0.06109259065289602</v>
+        <v>-0.06207343624960984</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.2396813277404249</v>
+        <v>0.2014079878245983</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.02200842463210253</v>
+        <v>0.01566473462830687</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.09589012055161014</v>
+        <v>0.09657544084306648</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.8739878441551753</v>
+        <v>0.8696725481069781</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.9341459088384783</v>
+        <v>0.9587453707113786</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.8268485078729834</v>
+        <v>0.8540436298634999</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.9415844976031479</v>
+        <v>0.8917191784513998</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.8043801496963014</v>
+        <v>0.8361938670098908</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.7553010704978103</v>
+        <v>0.848295464971081</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.8829952209424516</v>
+        <v>0.8722834729936295</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.1153522087331682</v>
+        <v>0.1218591693106626</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.283839471601818</v>
+        <v>0.2799155147094392</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.4000488166207219</v>
+        <v>0.2925582846961935</v>
       </c>
       <c r="AL9" t="n">
-        <v>1.547840153880537</v>
+        <v>1.330470625901064</v>
       </c>
       <c r="AM9" t="n">
-        <v>38.21542453709838</v>
+        <v>36.51039187147735</v>
       </c>
       <c r="AN9" t="n">
-        <v>0.6679078532527447</v>
+        <v>0.6311348585187539</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.1965305242038717</v>
+        <v>0.2104121732119549</v>
       </c>
       <c r="AP9" t="n">
-        <v>2.98801247819483</v>
+        <v>2.597582244513748</v>
       </c>
       <c r="AQ9" t="n">
-        <v>1879.438815024184</v>
+        <v>1568.614066941932</v>
       </c>
       <c r="AR9" t="n">
-        <v>6981.845262397033</v>
+        <v>7924.469878824059</v>
       </c>
       <c r="AS9" t="n">
-        <v>0.5196930735477172</v>
+        <v>0.4873691331859163</v>
       </c>
       <c r="AT9" t="n">
-        <v>0.3647370888905667</v>
+        <v>0.3598230414766896</v>
       </c>
       <c r="AU9" t="n">
-        <v>0.5282882503514874</v>
+        <v>0.5658625661684336</v>
       </c>
       <c r="AV9" t="n">
-        <v>11.45291907637547</v>
+        <v>9.867145310687034</v>
       </c>
       <c r="AW9" t="n">
-        <v>0.9044241731695122</v>
+        <v>0.9555207904420666</v>
       </c>
       <c r="AX9" t="n">
-        <v>1.338003512216513</v>
+        <v>1.325720617901662</v>
       </c>
       <c r="AY9" t="n">
-        <v>1.026419089056437</v>
+        <v>1.08144849817442</v>
       </c>
       <c r="AZ9" t="n">
-        <v>61.18651396075359</v>
+        <v>65.66449419727338</v>
       </c>
       <c r="BA9" t="n">
-        <v>0.239956293852658</v>
+        <v>0.221224367602786</v>
       </c>
       <c r="BB9" t="n">
-        <v>0.1489547861205378</v>
+        <v>0.1570946074007209</v>
       </c>
       <c r="BC9" t="n">
-        <v>1.023543306229923</v>
+        <v>1.05663176430806</v>
       </c>
       <c r="BD9" t="n">
-        <v>11.80173547336474</v>
+        <v>9.371896299749864</v>
       </c>
       <c r="BE9" t="n">
-        <v>4.376582971394909</v>
+        <v>3.578648432379639</v>
       </c>
       <c r="BF9" t="n">
-        <v>0.4306228749602797</v>
+        <v>0.7148790772735272</v>
       </c>
       <c r="BG9" t="n">
-        <v>0.09422009163112199</v>
+        <v>0.08204522570524243</v>
       </c>
       <c r="BH9" t="n">
-        <v>0.3865877097643577</v>
+        <v>0.4464979082602396</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.02040962732775814</v>
+        <v>0.0168056454697386</v>
       </c>
       <c r="BK9" t="n">
-        <v>92.16000256369774</v>
+        <v>92.28967013215856</v>
       </c>
       <c r="BL9" t="n">
-        <v>11.5023059483976</v>
+        <v>12.10742913426563</v>
       </c>
     </row>
     <row r="10">
@@ -2428,193 +2428,193 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>75807.68577717153</v>
+        <v>76052.72374803534</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2090380823488631</v>
+        <v>0.211862976381177</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3884716274060127</v>
+        <v>0.3604110850160335</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2115259821639954</v>
+        <v>0.1994187109729061</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1994739945041107</v>
+        <v>0.1999677290121636</v>
       </c>
       <c r="G10" t="n">
-        <v>0.04699064118697397</v>
+        <v>0.03595749755773835</v>
       </c>
       <c r="H10" t="n">
-        <v>320.7264701077852</v>
+        <v>321.8585378615632</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2709471839894276</v>
+        <v>0.2026579906630787</v>
       </c>
       <c r="J10" t="n">
-        <v>0.09852584854183725</v>
+        <v>0.1012148845706596</v>
       </c>
       <c r="K10" t="n">
-        <v>0.07560862838870219</v>
+        <v>0.1010106122946888</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1337213259702269</v>
+        <v>0.1536845418207198</v>
       </c>
       <c r="M10" t="n">
-        <v>0.9415152542705523</v>
+        <v>0.7390227250859409</v>
       </c>
       <c r="N10" t="n">
-        <v>0.4062199289575271</v>
+        <v>0.3294187588486901</v>
       </c>
       <c r="O10" t="n">
-        <v>0.09020718608547292</v>
+        <v>0.1070249566232446</v>
       </c>
       <c r="P10" t="n">
-        <v>1.038150885994387</v>
+        <v>1.34961179895692</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.906828811917163</v>
+        <v>0.843381868448169</v>
       </c>
       <c r="R10" t="n">
-        <v>1.013540031699452</v>
+        <v>0.9535871964857628</v>
       </c>
       <c r="S10" t="n">
-        <v>2.373042477549759</v>
+        <v>2.303713615451057</v>
       </c>
       <c r="T10" t="n">
-        <v>0.1481834765970744</v>
+        <v>0.1472284223475341</v>
       </c>
       <c r="U10" t="n">
-        <v>3.186488380196678</v>
+        <v>3.687207422321204</v>
       </c>
       <c r="V10" t="n">
-        <v>0.001247843023142831</v>
+        <v>0.001180877765453238</v>
       </c>
       <c r="W10" t="n">
-        <v>0.00239035198437692</v>
+        <v>0.002161233742029386</v>
       </c>
       <c r="X10" t="n">
-        <v>-0.04854210452931655</v>
+        <v>-0.0557183194531649</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.1975913831243319</v>
+        <v>0.2083004243920072</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.02228347240208872</v>
+        <v>0.01362970260320579</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.1035454393710499</v>
+        <v>0.1075891950533979</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.8365695530895042</v>
+        <v>0.8380626443816566</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.9451082863250163</v>
+        <v>0.9553831954705395</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.8873962865906384</v>
+        <v>0.8267508061607378</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.8564989855661035</v>
+        <v>0.8988056751580498</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.8154260705477543</v>
+        <v>0.7839757886572484</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.8269950450585433</v>
+        <v>0.7825259938080801</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.7693790496022315</v>
+        <v>0.8077185519175154</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.1116959246208749</v>
+        <v>0.0924147347685374</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.3404796897618677</v>
+        <v>0.2716354018445912</v>
       </c>
       <c r="AK10" t="n">
-        <v>0.356986234738404</v>
+        <v>0.3468062860302326</v>
       </c>
       <c r="AL10" t="n">
-        <v>1.61494525845166</v>
+        <v>1.297331875938055</v>
       </c>
       <c r="AM10" t="n">
-        <v>26.8500477813434</v>
+        <v>33.88007608780344</v>
       </c>
       <c r="AN10" t="n">
-        <v>0.6512777935385762</v>
+        <v>0.5635276716981547</v>
       </c>
       <c r="AO10" t="n">
-        <v>0.177862001002111</v>
+        <v>0.2274301435663959</v>
       </c>
       <c r="AP10" t="n">
-        <v>2.826325438895728</v>
+        <v>2.85685203908911</v>
       </c>
       <c r="AQ10" t="n">
-        <v>1646.802575592755</v>
+        <v>1758.797781838484</v>
       </c>
       <c r="AR10" t="n">
-        <v>8250.280145305887</v>
+        <v>8079.168458048948</v>
       </c>
       <c r="AS10" t="n">
-        <v>0.4650554591279565</v>
+        <v>0.5157927599143419</v>
       </c>
       <c r="AT10" t="n">
-        <v>0.3571996310200458</v>
+        <v>0.3339090904151558</v>
       </c>
       <c r="AU10" t="n">
-        <v>0.5866449645881191</v>
+        <v>0.6324166046013371</v>
       </c>
       <c r="AV10" t="n">
-        <v>9.538448118748221</v>
+        <v>9.408089131797043</v>
       </c>
       <c r="AW10" t="n">
-        <v>0.9752264264993795</v>
+        <v>1.039921975800926</v>
       </c>
       <c r="AX10" t="n">
-        <v>1.261572105656576</v>
+        <v>1.462811689451607</v>
       </c>
       <c r="AY10" t="n">
-        <v>1.11588186398092</v>
+        <v>0.9482212633155058</v>
       </c>
       <c r="AZ10" t="n">
-        <v>59.38172285024977</v>
+        <v>63.67582643430633</v>
       </c>
       <c r="BA10" t="n">
-        <v>0.227103839188819</v>
+        <v>0.2391658188111264</v>
       </c>
       <c r="BB10" t="n">
-        <v>0.1543689466303162</v>
+        <v>0.188464496885523</v>
       </c>
       <c r="BC10" t="n">
-        <v>1.071747300390987</v>
+        <v>1.036150582043138</v>
       </c>
       <c r="BD10" t="n">
-        <v>11.17744008537902</v>
+        <v>10.68449135151276</v>
       </c>
       <c r="BE10" t="n">
-        <v>3.362176761146378</v>
+        <v>3.942155424734493</v>
       </c>
       <c r="BF10" t="n">
-        <v>0.247330846981989</v>
+        <v>0.4223124724650876</v>
       </c>
       <c r="BG10" t="n">
-        <v>0.09651830027839924</v>
+        <v>0.09002468159397432</v>
       </c>
       <c r="BH10" t="n">
-        <v>0.4460190283171462</v>
+        <v>0.4134473706445501</v>
       </c>
       <c r="BI10" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="BJ10" t="n">
-        <v>0.02119587159902278</v>
+        <v>0.01986769092823636</v>
       </c>
       <c r="BK10" t="n">
-        <v>95.5037500791131</v>
+        <v>85.11976582561658</v>
       </c>
       <c r="BL10" t="n">
-        <v>13.38404434021309</v>
+        <v>11.72813548183283</v>
       </c>
     </row>
     <row r="11">
@@ -2622,193 +2622,193 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>84836.55124948265</v>
+        <v>86724.84738470631</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1772409550030191</v>
+        <v>0.1980612341443672</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3717666352489247</v>
+        <v>0.3685886366285247</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2079818798666994</v>
+        <v>0.213121200063708</v>
       </c>
       <c r="F11" t="n">
-        <v>0.201366767027255</v>
+        <v>0.205796999646691</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0583178244826885</v>
+        <v>0.0487523222892613</v>
       </c>
       <c r="H11" t="n">
-        <v>322.8088236672816</v>
+        <v>332.5573563797357</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2093970988628202</v>
+        <v>0.1896928845580457</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0850617050602146</v>
+        <v>0.08506644905053587</v>
       </c>
       <c r="K11" t="n">
-        <v>0.09474321671149886</v>
+        <v>0.07837893734392284</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1555754399666149</v>
+        <v>0.1371239220133107</v>
       </c>
       <c r="M11" t="n">
-        <v>0.7861384810930234</v>
+        <v>0.7999692971979123</v>
       </c>
       <c r="N11" t="n">
-        <v>0.3416783969252369</v>
+        <v>0.4402102842974812</v>
       </c>
       <c r="O11" t="n">
-        <v>0.1046230991362246</v>
+        <v>0.1139278298211041</v>
       </c>
       <c r="P11" t="n">
-        <v>1.402398184669897</v>
+        <v>1.018285543092097</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.9294993646074079</v>
+        <v>1.094854774133981</v>
       </c>
       <c r="R11" t="n">
-        <v>0.9579078808243369</v>
+        <v>1.03157650984655</v>
       </c>
       <c r="S11" t="n">
-        <v>1.741742843564659</v>
+        <v>2.539200769361178</v>
       </c>
       <c r="T11" t="n">
-        <v>0.1529183647970566</v>
+        <v>0.1240788635300343</v>
       </c>
       <c r="U11" t="n">
-        <v>3.709864635182948</v>
+        <v>3.350567973848703</v>
       </c>
       <c r="V11" t="n">
-        <v>0.001064686279366211</v>
+        <v>0.001013137021210395</v>
       </c>
       <c r="W11" t="n">
-        <v>0.002303301460126671</v>
+        <v>0.002172531606039941</v>
       </c>
       <c r="X11" t="n">
-        <v>-0.05737631976757335</v>
+        <v>-0.05754705565231732</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.183264185527874</v>
+        <v>0.2119706076671964</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.02427608330212391</v>
+        <v>0.02209384541925965</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.1008734581965116</v>
+        <v>0.09937325728100424</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.942189930017173</v>
+        <v>0.79893225718943</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.9180584077561497</v>
+        <v>0.9510253537608475</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.8495957160474044</v>
+        <v>0.8745401417706864</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.8728475218530153</v>
+        <v>0.9070597364329525</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.8186307093918104</v>
+        <v>0.7966766673790306</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.8666305184439824</v>
+        <v>0.7966340363540739</v>
       </c>
       <c r="AH11" t="n">
-        <v>0.913389592548926</v>
+        <v>0.7964262957677187</v>
       </c>
       <c r="AI11" t="n">
-        <v>0.1030079353064415</v>
+        <v>0.1131131762401585</v>
       </c>
       <c r="AJ11" t="n">
-        <v>0.2946356009441223</v>
+        <v>0.3082941781163837</v>
       </c>
       <c r="AK11" t="n">
-        <v>0.3662682925801036</v>
+        <v>0.3956375150276801</v>
       </c>
       <c r="AL11" t="n">
-        <v>1.391327765339252</v>
+        <v>1.595847953234814</v>
       </c>
       <c r="AM11" t="n">
-        <v>31.76994832596433</v>
+        <v>26.73540383998976</v>
       </c>
       <c r="AN11" t="n">
-        <v>0.5141498958244761</v>
+        <v>0.6726700740991098</v>
       </c>
       <c r="AO11" t="n">
-        <v>0.2029500579010021</v>
+        <v>0.218965389263307</v>
       </c>
       <c r="AP11" t="n">
-        <v>2.666731760458289</v>
+        <v>3.1600554564288</v>
       </c>
       <c r="AQ11" t="n">
-        <v>1976.784186286478</v>
+        <v>1850.024984714394</v>
       </c>
       <c r="AR11" t="n">
-        <v>8052.452874165509</v>
+        <v>8626.841084068868</v>
       </c>
       <c r="AS11" t="n">
-        <v>0.4495385753477266</v>
+        <v>0.5721001011796749</v>
       </c>
       <c r="AT11" t="n">
-        <v>0.3513390987217835</v>
+        <v>0.3696115509009785</v>
       </c>
       <c r="AU11" t="n">
-        <v>0.5740338000473271</v>
+        <v>0.5065225763735883</v>
       </c>
       <c r="AV11" t="n">
-        <v>10.35563875347649</v>
+        <v>10.11348142493863</v>
       </c>
       <c r="AW11" t="n">
-        <v>0.8640253751186981</v>
+        <v>1.107949587188444</v>
       </c>
       <c r="AX11" t="n">
-        <v>1.385154784034286</v>
+        <v>1.37819350568418</v>
       </c>
       <c r="AY11" t="n">
-        <v>1.039279674733104</v>
+        <v>1.010002777427175</v>
       </c>
       <c r="AZ11" t="n">
-        <v>48.72812224763465</v>
+        <v>60.50940599272992</v>
       </c>
       <c r="BA11" t="n">
-        <v>0.2639858791452677</v>
+        <v>0.2345223858876023</v>
       </c>
       <c r="BB11" t="n">
-        <v>0.1914802280068888</v>
+        <v>0.1754707887476065</v>
       </c>
       <c r="BC11" t="n">
-        <v>1.027296779714829</v>
+        <v>1.063399499271189</v>
       </c>
       <c r="BD11" t="n">
-        <v>11.28879782531936</v>
+        <v>9.905896851755855</v>
       </c>
       <c r="BE11" t="n">
-        <v>3.867735155650715</v>
+        <v>4.279115033765054</v>
       </c>
       <c r="BF11" t="n">
-        <v>0.7914296007817012</v>
+        <v>0.5057783168942878</v>
       </c>
       <c r="BG11" t="n">
-        <v>0.08827929218944659</v>
+        <v>0.09947297335867367</v>
       </c>
       <c r="BH11" t="n">
-        <v>0.4102041907259453</v>
+        <v>0.3560763373323174</v>
       </c>
       <c r="BI11" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="BJ11" t="n">
-        <v>0.01857223918479103</v>
+        <v>0.01827374948597979</v>
       </c>
       <c r="BK11" t="n">
-        <v>85.36119572420895</v>
+        <v>77.70446126276917</v>
       </c>
       <c r="BL11" t="n">
-        <v>11.86575144417808</v>
+        <v>11.97968652663782</v>
       </c>
     </row>
     <row r="12">
@@ -2816,193 +2816,193 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>77429.54808562709</v>
+        <v>90749.52846293339</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2206349661274482</v>
+        <v>0.2059224580395067</v>
       </c>
       <c r="D12" t="n">
-        <v>0.360705001666726</v>
+        <v>0.368079700401921</v>
       </c>
       <c r="E12" t="n">
-        <v>0.200910369238065</v>
+        <v>0.2051384964536189</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2042972539967521</v>
+        <v>0.2037607334109072</v>
       </c>
       <c r="G12" t="n">
-        <v>0.04120176185892341</v>
+        <v>0.044720015147688</v>
       </c>
       <c r="H12" t="n">
-        <v>316.7889448809097</v>
+        <v>325.6501523245338</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1988178659326675</v>
+        <v>0.2180301051525202</v>
       </c>
       <c r="J12" t="n">
-        <v>0.112095193021529</v>
+        <v>0.1115681192159465</v>
       </c>
       <c r="K12" t="n">
-        <v>0.09581275908580149</v>
+        <v>0.09032396054672752</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1173047609726833</v>
+        <v>0.1685338980972898</v>
       </c>
       <c r="M12" t="n">
-        <v>0.8832484662859844</v>
+        <v>0.866464099126379</v>
       </c>
       <c r="N12" t="n">
-        <v>0.4680320605616838</v>
+        <v>0.3732671644090462</v>
       </c>
       <c r="O12" t="n">
-        <v>0.09292233528386178</v>
+        <v>0.11081233178915</v>
       </c>
       <c r="P12" t="n">
-        <v>1.00148572304863</v>
+        <v>1.411616216676614</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.067996144381847</v>
+        <v>1.022420247810777</v>
       </c>
       <c r="R12" t="n">
-        <v>0.9331609845210842</v>
+        <v>0.9074217028309082</v>
       </c>
       <c r="S12" t="n">
-        <v>2.264063555147379</v>
+        <v>1.763221378910395</v>
       </c>
       <c r="T12" t="n">
-        <v>0.1292720951710966</v>
+        <v>0.1447691873583171</v>
       </c>
       <c r="U12" t="n">
-        <v>4.020058696876928</v>
+        <v>3.926830637154561</v>
       </c>
       <c r="V12" t="n">
-        <v>0.001076365508794658</v>
+        <v>0.001091558156297214</v>
       </c>
       <c r="W12" t="n">
-        <v>0.002520389286883899</v>
+        <v>0.002340747757360137</v>
       </c>
       <c r="X12" t="n">
-        <v>-0.06368804999180651</v>
+        <v>-0.04615396685803116</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.2004062891453814</v>
+        <v>0.2213838742169549</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.01526829057741712</v>
+        <v>0.02491998274639671</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.09197072573633246</v>
+        <v>0.1003503332774144</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.913273456496013</v>
+        <v>0.8783275126672061</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.9383442381294483</v>
+        <v>0.9419122051151525</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.8216106568273117</v>
+        <v>0.8448845074047305</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.9029817875678119</v>
+        <v>0.8816817195731537</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.7982903347060238</v>
+        <v>0.7705510752935529</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.7421980184645999</v>
+        <v>0.7354390115009087</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.8183534905491777</v>
+        <v>0.9033966674535834</v>
       </c>
       <c r="AI12" t="n">
-        <v>0.09869942280716766</v>
+        <v>0.1040814092782831</v>
       </c>
       <c r="AJ12" t="n">
-        <v>0.2576730367512008</v>
+        <v>0.2879106103806051</v>
       </c>
       <c r="AK12" t="n">
-        <v>0.3464435473875559</v>
+        <v>0.3385356545319901</v>
       </c>
       <c r="AL12" t="n">
-        <v>1.230585767791799</v>
+        <v>1.404265323824252</v>
       </c>
       <c r="AM12" t="n">
-        <v>33.34088724542656</v>
+        <v>29.8144315069137</v>
       </c>
       <c r="AN12" t="n">
-        <v>0.6114946643780015</v>
+        <v>0.6080969361455687</v>
       </c>
       <c r="AO12" t="n">
-        <v>0.1928925936562224</v>
+        <v>0.1959469044364472</v>
       </c>
       <c r="AP12" t="n">
-        <v>2.840754954025904</v>
+        <v>2.551873840156013</v>
       </c>
       <c r="AQ12" t="n">
-        <v>1813.359996372491</v>
+        <v>1891.538894991504</v>
       </c>
       <c r="AR12" t="n">
-        <v>7542.449893152141</v>
+        <v>8263.290240877532</v>
       </c>
       <c r="AS12" t="n">
-        <v>0.5597708244275359</v>
+        <v>0.4642824689595264</v>
       </c>
       <c r="AT12" t="n">
-        <v>0.3627399422990216</v>
+        <v>0.3574283457191614</v>
       </c>
       <c r="AU12" t="n">
-        <v>0.5555248466415805</v>
+        <v>0.6065390835053921</v>
       </c>
       <c r="AV12" t="n">
-        <v>10.15965798946419</v>
+        <v>11.69296793937919</v>
       </c>
       <c r="AW12" t="n">
-        <v>1.089413416819823</v>
+        <v>1.002424654490542</v>
       </c>
       <c r="AX12" t="n">
-        <v>1.409969673487432</v>
+        <v>1.267548281839412</v>
       </c>
       <c r="AY12" t="n">
-        <v>1.143561322282757</v>
+        <v>1.001476239734631</v>
       </c>
       <c r="AZ12" t="n">
-        <v>53.82187338670879</v>
+        <v>60.74260127203655</v>
       </c>
       <c r="BA12" t="n">
-        <v>0.2182410921628411</v>
+        <v>0.2071979281958868</v>
       </c>
       <c r="BB12" t="n">
-        <v>0.1641265697606655</v>
+        <v>0.1653887270798456</v>
       </c>
       <c r="BC12" t="n">
-        <v>1.043381927829895</v>
+        <v>0.944487578430343</v>
       </c>
       <c r="BD12" t="n">
-        <v>12.68489743124014</v>
+        <v>11.04044053860102</v>
       </c>
       <c r="BE12" t="n">
-        <v>5.117637118845081</v>
+        <v>4.750935279627871</v>
       </c>
       <c r="BF12" t="n">
-        <v>0.9763075083580499</v>
+        <v>0.7264566419835317</v>
       </c>
       <c r="BG12" t="n">
-        <v>0.07917383867261189</v>
+        <v>0.08694230759247783</v>
       </c>
       <c r="BH12" t="n">
-        <v>0.4647362437220499</v>
+        <v>0.3954558458510583</v>
       </c>
       <c r="BI12" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="BJ12" t="n">
-        <v>0.01931369728869046</v>
+        <v>0.01948226081722156</v>
       </c>
       <c r="BK12" t="n">
-        <v>84.13420755807149</v>
+        <v>84.78022263534477</v>
       </c>
       <c r="BL12" t="n">
-        <v>10.48058735748711</v>
+        <v>13.46235400617559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>